<commit_message>
fix(excel2xml): prevent writing empty text-prop, make text-prop validation less restrictive (DEV-1440) #243
</commit_message>
<xml_diff>
--- a/testdata/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml-testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11144152-9CDA-4F48-96A9-C4EBC81BFC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB0E0CE-89D2-714E-AB1E-611B19505BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10380" yWindow="-21100" windowWidth="49140" windowHeight="21100" xr2:uid="{8DC9C588-8EAF-9149-8D6F-E65826635888}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8DC9C588-8EAF-9149-8D6F-E65826635888}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
   <si>
     <t>id</t>
   </si>
@@ -845,6 +845,12 @@
   <si>
     <t>#5d1f1e</t>
   </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
@@ -1016,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1042,6 +1048,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B59957-CA62-894B-8744-01ADFD605729}">
   <dimension ref="A1:RN44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2844,7 +2851,25 @@
         <v>29</v>
       </c>
       <c r="T3" s="7"/>
+      <c r="U3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="X3" s="7"/>
+      <c r="Y3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="AB3" s="7"/>
       <c r="AC3"/>
       <c r="AD3"/>

</xml_diff>

<commit_message>
fix(xmlupload): improve URL recognition (DEV-1557) (#266)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml-testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB0E0CE-89D2-714E-AB1E-611B19505BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D4EAF-34A2-174B-B0AE-B44196716646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8DC9C588-8EAF-9149-8D6F-E65826635888}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="example" localSheetId="0">Sheet1!$A$1:$PF$32</definedName>
+    <definedName name="example" localSheetId="0">Sheet1!$A$1:$PF$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="140">
   <si>
     <t>id</t>
   </si>
@@ -629,13 +629,7 @@
     <t>uri-prop</t>
   </si>
   <si>
-    <t>http://d-nb.info/gnd/11855333X</t>
-  </si>
-  <si>
     <t>:hasExternalLink</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Homer</t>
   </si>
   <si>
     <t>annotation_0</t>
@@ -851,12 +845,72 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>https://reg-exr.com:3000/path/to/file_(%C3%89).htm</t>
+  </si>
+  <si>
+    <t>https://en.wiktionary.org/wiki/Ῥόδος</t>
+  </si>
+  <si>
+    <t>https://www.test-case.ch/</t>
+  </si>
+  <si>
+    <t>https://reg-exr.com:3000</t>
+  </si>
+  <si>
+    <t>https://reg-exr.com:3000/path/to/file#fragment</t>
+  </si>
+  <si>
+    <t>https://reg-exr.com:3000/path/to/file?query=test</t>
+  </si>
+  <si>
+    <t>https://reg-exr.com:3000/path/to/file?query=test#fragment</t>
+  </si>
+  <si>
+    <t>https://reg-exr.com/path/to/file?query=test#fragment</t>
+  </si>
+  <si>
+    <t>:hasAnotherLink</t>
+  </si>
+  <si>
+    <t>http://www.168.1.1.0/path</t>
+  </si>
+  <si>
+    <t>http://www.168.1.1.0:4200/path</t>
+  </si>
+  <si>
+    <t>http://[2001:0db8:0000:0000:0000:8a2e:0370:7334]:4200/path</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Haiku#/media/File:Basho_Horohoroto.jpg</t>
+  </si>
+  <si>
+    <t>:hasThirdLink</t>
+  </si>
+  <si>
+    <t>http://datypic.com/prod.html#shirt</t>
+  </si>
+  <si>
+    <t>https://www.findagrave.com/memorial/171722836/krikor-madenician?_gl=1*100n0s5*_ga*NzIzMDQxNjc2LjE2Mjg2MDk1OTQ.*_ga_4QT8FMEX30*MTY1Mjc5OTI4OC4xNC4xLjE2NTI4MDA2MDQuMA..</t>
+  </si>
+  <si>
+    <t>https://markarslan.org/ArmenianImmigrants/Public-ViewDetail-ArmenianImmigrants-Main.php?submit=View&amp;Staging=&amp;SourcePage=Public-ViewSummary-ArmenianImmigrants-Main-ByDestinationDate&amp;SelectDestinationYear=1907&amp;SelectLastNameStd=all&amp;argument1=PLIN-29NOV1907-3-73-0018</t>
+  </si>
+  <si>
+    <t>http://markarslan.org/ArmenianImmigrants/Public-ViewDetail-ArmenianImmigrants-Main.php?submit=View&amp;Staging=&amp;SourcePage=Public-ViewSummary-ArmenianImmigrants-Main-ByDestinationDate&amp;SelectDestinationYear=1907&amp;SelectLastNameStd=all&amp;argument1=CRTH-12JAN1907-3-%404-0016</t>
+  </si>
+  <si>
+    <t>https://www.ancestry.com/discoveryui-content/view/47577828:60525?ssrc=pt&amp;tid=109007397&amp;pid=410070328478</t>
+  </si>
+  <si>
+    <t>:hasFourthLink</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -880,6 +934,14 @@
     </font>
     <font>
       <sz val="11.3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1019,10 +1081,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1049,8 +1112,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1367,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B59957-CA62-894B-8744-01ADFD605729}">
-  <dimension ref="A1:RN44"/>
+  <dimension ref="A1:RN47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1813,10 +1881,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1825,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
@@ -1885,7 +1953,7 @@
         <v>24</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AD1"/>
       <c r="AE1"/>
@@ -1893,7 +1961,7 @@
       <c r="AG1"/>
       <c r="AH1"/>
       <c r="AI1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AJ1"/>
       <c r="AK1"/>
@@ -2354,7 +2422,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>25</v>
@@ -2367,7 +2435,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2"/>
       <c r="AD2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AE2"/>
       <c r="AF2"/>
@@ -2842,7 +2910,7 @@
       </c>
       <c r="P3" s="7"/>
       <c r="Q3" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>28</v>
@@ -2852,7 +2920,7 @@
       </c>
       <c r="T3" s="7"/>
       <c r="U3" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>28</v>
@@ -2862,7 +2930,7 @@
       </c>
       <c r="X3" s="7"/>
       <c r="Y3" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>28</v>
@@ -2874,7 +2942,7 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AF3"/>
       <c r="AG3"/>
@@ -3337,15 +3405,33 @@
         <v>51</v>
       </c>
       <c r="L4" s="7"/>
-      <c r="M4" s="8" t="s">
-        <v>52</v>
+      <c r="M4" t="s">
+        <v>121</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="7"/>
+      <c r="Q4" t="s">
+        <v>122</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="T4" s="7"/>
+      <c r="U4" t="s">
+        <v>123</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="X4" s="7"/>
+      <c r="Y4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="AB4" s="7"/>
       <c r="AC4"/>
       <c r="AD4"/>
@@ -3802,43 +3888,43 @@
       <c r="RM4"/>
       <c r="RN4"/>
     </row>
-    <row r="5" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="10" t="s">
+    <row r="5" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I5" s="7"/>
+      <c r="J5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="11"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="7"/>
+      <c r="U5" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB5" s="7"/>
       <c r="AC5"/>
       <c r="AD5"/>
       <c r="AE5"/>
@@ -4295,33 +4381,47 @@
       <c r="RN5"/>
     </row>
     <row r="6" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="I6" s="7"/>
+      <c r="J6" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="L6" s="7"/>
+      <c r="M6" t="s">
+        <v>129</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="P6" s="7"/>
+      <c r="Q6" t="s">
+        <v>130</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="T6" s="7"/>
+      <c r="U6" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="X6" s="7"/>
+      <c r="Y6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA6" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="AB6" s="7"/>
       <c r="AC6"/>
-      <c r="AD6" t="s">
-        <v>117</v>
-      </c>
+      <c r="AD6"/>
       <c r="AE6"/>
       <c r="AF6"/>
-      <c r="AG6" t="s">
-        <v>116</v>
-      </c>
+      <c r="AG6"/>
       <c r="AH6"/>
       <c r="AI6"/>
       <c r="AJ6"/>
@@ -4775,24 +4875,39 @@
     <row r="7" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I7" s="7"/>
       <c r="J7" s="6" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="L7" s="7"/>
-      <c r="M7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>28</v>
+      <c r="M7" t="s">
+        <v>134</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P7" s="7"/>
+      <c r="Q7" t="s">
+        <v>135</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="T7" s="7"/>
+      <c r="U7" t="s">
+        <v>136</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="X7" s="7"/>
+      <c r="Y7" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="AB7" s="7"/>
       <c r="AC7"/>
       <c r="AD7"/>
@@ -5259,23 +5374,33 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O8" s="6" t="s">
+      <c r="J8" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="AB8" s="7"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="11"/>
       <c r="AC8"/>
       <c r="AD8"/>
       <c r="AE8"/>
@@ -5733,47 +5858,32 @@
     </row>
     <row r="9" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="16"/>
+      <c r="I9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="AB9" s="7"/>
       <c r="AC9"/>
-      <c r="AD9"/>
+      <c r="AD9" t="s">
+        <v>115</v>
+      </c>
       <c r="AE9"/>
       <c r="AF9"/>
-      <c r="AG9"/>
+      <c r="AG9" t="s">
+        <v>114</v>
+      </c>
       <c r="AH9"/>
       <c r="AI9"/>
       <c r="AJ9"/>
@@ -6227,14 +6337,14 @@
     <row r="10" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I10" s="7"/>
       <c r="J10" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>27</v>
       </c>
       <c r="L10" s="7"/>
-      <c r="M10" s="17" t="s">
-        <v>77</v>
+      <c r="M10" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>28</v>
@@ -6243,15 +6353,10 @@
         <v>29</v>
       </c>
       <c r="P10" s="7"/>
-      <c r="Q10" s="17"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="17"/>
       <c r="X10" s="7"/>
-      <c r="Y10" s="17"/>
       <c r="AB10" s="7"/>
-      <c r="AC10" t="s">
-        <v>118</v>
-      </c>
+      <c r="AC10"/>
       <c r="AD10"/>
       <c r="AE10"/>
       <c r="AF10"/>
@@ -6706,30 +6811,32 @@
       <c r="RM10"/>
       <c r="RN10"/>
     </row>
-    <row r="11" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I11" s="7"/>
+    <row r="11" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L11" s="7"/>
-      <c r="M11" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>31</v>
+      <c r="M11" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="O11" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P11" s="7"/>
-      <c r="Q11" s="17"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="17"/>
       <c r="X11" s="7"/>
-      <c r="Y11" s="17"/>
       <c r="AB11" s="7"/>
       <c r="AC11"/>
       <c r="AD11"/>
@@ -7187,30 +7294,43 @@
       <c r="RN11"/>
     </row>
     <row r="12" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I12" s="7"/>
-      <c r="J12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="6" t="s">
+      <c r="A12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="17"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="17"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="17"/>
-      <c r="AB12" s="7"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="16"/>
       <c r="AC12"/>
       <c r="AD12"/>
       <c r="AE12"/>
@@ -7666,39 +7786,34 @@
       <c r="RM12"/>
       <c r="RN12"/>
     </row>
-    <row r="13" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10" t="s">
+    <row r="13" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="7"/>
+      <c r="J13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="10"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="17"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="17"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="17"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" t="s">
+        <v>116</v>
+      </c>
       <c r="AD13"/>
       <c r="AE13"/>
       <c r="AF13"/>
@@ -8154,44 +8269,30 @@
       <c r="RN13"/>
     </row>
     <row r="14" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="15"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="16"/>
+      <c r="J14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="17"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="17"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="17"/>
+      <c r="AB14" s="7"/>
       <c r="AC14"/>
       <c r="AD14"/>
       <c r="AE14"/>
@@ -8648,27 +8749,29 @@
       <c r="RN14"/>
     </row>
     <row r="15" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="8" t="s">
-        <v>40</v>
+      <c r="J15" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="L15" s="7"/>
-      <c r="M15" s="8" t="s">
-        <v>89</v>
+      <c r="M15" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O15" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P15" s="7"/>
+      <c r="Q15" s="17"/>
       <c r="T15" s="7"/>
+      <c r="U15" s="17"/>
       <c r="X15" s="7"/>
+      <c r="Y15" s="17"/>
       <c r="AB15" s="7"/>
       <c r="AC15"/>
       <c r="AD15"/>
@@ -9126,39 +9229,34 @@
       <c r="RN15"/>
     </row>
     <row r="16" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="12" t="s">
-        <v>41</v>
+      <c r="J16" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="12" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="N16" s="10"/>
-      <c r="O16" s="12" t="s">
+      <c r="O16" s="10" t="s">
         <v>29</v>
       </c>
       <c r="P16" s="11"/>
-      <c r="Q16" s="10"/>
+      <c r="Q16" s="13"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="11"/>
-      <c r="U16" s="10"/>
+      <c r="U16" s="13"/>
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
       <c r="X16" s="11"/>
-      <c r="Y16" s="10"/>
+      <c r="Y16" s="13"/>
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
       <c r="AB16" s="11"/>
@@ -9618,28 +9716,44 @@
       <c r="RN16"/>
     </row>
     <row r="17" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17"/>
-      <c r="G17" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="A17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="15"/>
       <c r="I17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="AB17" s="7"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="16"/>
       <c r="AC17"/>
       <c r="AD17"/>
       <c r="AE17"/>
@@ -10096,33 +10210,25 @@
       <c r="RN17"/>
     </row>
     <row r="18" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17"/>
       <c r="I18" s="7"/>
       <c r="J18" s="8" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>27</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>28</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="P18" s="7"/>
-      <c r="Q18" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S18" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="T18" s="7"/>
       <c r="X18" s="7"/>
       <c r="AB18" s="7"/>
@@ -10581,25 +10687,43 @@
       <c r="RM18"/>
       <c r="RN18"/>
     </row>
-    <row r="19" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I19" s="7"/>
-      <c r="J19" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="AB19" s="7"/>
+    <row r="19" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" s="10"/>
+      <c r="O19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="11"/>
       <c r="AC19"/>
       <c r="AD19"/>
       <c r="AE19"/>
@@ -11056,20 +11180,24 @@
       <c r="RN19"/>
     </row>
     <row r="20" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="I20" s="7"/>
-      <c r="J20" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="L20" s="7"/>
-      <c r="M20" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="P20" s="7"/>
       <c r="T20" s="7"/>
       <c r="X20" s="7"/>
@@ -11529,25 +11657,34 @@
       <c r="RM20"/>
       <c r="RN20"/>
     </row>
-    <row r="21" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="I21" s="11"/>
+    <row r="21" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="7"/>
       <c r="J21" s="8" t="s">
-        <v>94</v>
+        <v>26</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="8" t="s">
-        <v>75</v>
+        <v>88</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P21" s="7"/>
+      <c r="Q21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="T21" s="7"/>
       <c r="X21" s="7"/>
       <c r="AB21" s="7"/>
@@ -12007,46 +12144,24 @@
       <c r="RN21"/>
     </row>
     <row r="22" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>86</v>
-      </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="16"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="16"/>
+      <c r="J22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="AB22" s="7"/>
       <c r="AC22"/>
       <c r="AD22"/>
       <c r="AE22"/>
@@ -12503,34 +12618,21 @@
       <c r="RN22"/>
     </row>
     <row r="23" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
       <c r="I23" s="7"/>
       <c r="J23" s="8" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="L23" s="7"/>
       <c r="M23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="O23" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="N23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="P23" s="7"/>
-      <c r="Q23" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S23" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="T23" s="7"/>
       <c r="X23" s="7"/>
       <c r="AB23" s="7"/>
@@ -12989,45 +13091,26 @@
       <c r="RM23"/>
       <c r="RN23"/>
     </row>
-    <row r="24" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="17"/>
-      <c r="I24" s="7"/>
+    <row r="24" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="I24" s="11"/>
       <c r="J24" s="8" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L24" s="7"/>
       <c r="M24" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="O24" s="6" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="P24" s="7"/>
-      <c r="Q24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="R24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="S24" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="T24" s="7"/>
-      <c r="U24" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="W24" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="X24" s="7"/>
       <c r="AB24" s="7"/>
       <c r="AC24"/>
@@ -13486,25 +13569,46 @@
       <c r="RN24"/>
     </row>
     <row r="25" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
+      <c r="A25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>84</v>
+      </c>
       <c r="I25" s="7"/>
-      <c r="J25" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" s="7"/>
-      <c r="M25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="X25" s="7"/>
-      <c r="AB25" s="7"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="15"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="16"/>
       <c r="AC25"/>
       <c r="AD25"/>
       <c r="AE25"/>
@@ -13964,19 +14068,31 @@
       <c r="A26" s="17"/>
       <c r="I26" s="7"/>
       <c r="J26" s="8" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="L26" s="7"/>
-      <c r="M26" s="9" t="s">
-        <v>71</v>
+      <c r="M26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P26" s="7"/>
+      <c r="Q26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="R26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S26" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="T26" s="7"/>
       <c r="X26" s="7"/>
       <c r="AB26" s="7"/>
@@ -14439,28 +14555,37 @@
       <c r="A27" s="17"/>
       <c r="I27" s="7"/>
       <c r="J27" s="8" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="L27" s="7"/>
       <c r="M27" s="8" t="s">
-        <v>72</v>
+        <v>63</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="8" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="R27" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T27" s="7"/>
-      <c r="U27" s="6">
-        <v>2022</v>
+      <c r="U27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="V27" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="W27" s="6" t="s">
         <v>29</v>
@@ -14922,43 +15047,26 @@
       <c r="RM27"/>
       <c r="RN27"/>
     </row>
-    <row r="28" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="10">
-        <v>4711</v>
-      </c>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10" t="s">
+    <row r="28" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="17"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="O28" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="10"/>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="10"/>
-      <c r="AB28" s="11"/>
+      <c r="P28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="AB28" s="7"/>
       <c r="AC28"/>
       <c r="AD28"/>
       <c r="AE28"/>
@@ -15415,23 +15523,21 @@
       <c r="RN28"/>
     </row>
     <row r="29" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="A29" s="17"/>
       <c r="I29" s="7"/>
+      <c r="J29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="L29" s="7"/>
+      <c r="M29" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="P29" s="7"/>
       <c r="T29" s="7"/>
       <c r="X29" s="7"/>
@@ -15892,31 +15998,39 @@
       <c r="RN29"/>
     </row>
     <row r="30" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="6" t="s">
-        <v>26</v>
+      <c r="J30" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="L30" s="7"/>
-      <c r="M30" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>28</v>
+      <c r="M30" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="O30" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P30" s="7"/>
+      <c r="Q30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="T30" s="7"/>
+      <c r="U30" s="6">
+        <v>2022</v>
+      </c>
+      <c r="W30" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="X30" s="7"/>
       <c r="AB30" s="7"/>
       <c r="AC30"/>
-      <c r="AD30" t="s">
-        <v>116</v>
-      </c>
+      <c r="AD30"/>
       <c r="AE30"/>
       <c r="AF30"/>
       <c r="AG30"/>
@@ -16371,7 +16485,7 @@
       <c r="RN30"/>
     </row>
     <row r="31" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="A31" s="13"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
@@ -16380,32 +16494,34 @@
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
       <c r="I31" s="11"/>
-      <c r="J31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L31" s="7"/>
-      <c r="M31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="O31" s="6" t="s">
+      <c r="J31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="10">
+        <v>4711</v>
+      </c>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="S31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T31" s="7"/>
-      <c r="X31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" t="s">
-        <v>118</v>
-      </c>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="10"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="10"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31"/>
       <c r="AD31"/>
       <c r="AE31"/>
       <c r="AF31"/>
@@ -16862,37 +16978,27 @@
     </row>
     <row r="32" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="15"/>
-      <c r="AB32" s="15"/>
-      <c r="AC32" t="s">
-        <v>115</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32"/>
       <c r="AD32"/>
       <c r="AE32"/>
       <c r="AF32"/>
@@ -17347,38 +17453,1494 @@
       <c r="RM32"/>
       <c r="RN32"/>
     </row>
-    <row r="33" spans="2:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="33" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="7"/>
+      <c r="J33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L33" s="7"/>
+      <c r="M33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="N33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33"/>
+      <c r="AD33" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+      <c r="AL33"/>
+      <c r="AM33"/>
+      <c r="AN33"/>
+      <c r="AO33"/>
+      <c r="AP33"/>
+      <c r="AQ33"/>
+      <c r="AR33"/>
+      <c r="AS33"/>
+      <c r="AT33"/>
+      <c r="AU33"/>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33"/>
+      <c r="AY33"/>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
+      <c r="BC33"/>
+      <c r="BD33"/>
+      <c r="BE33"/>
+      <c r="BF33"/>
+      <c r="BG33"/>
+      <c r="BH33"/>
+      <c r="BI33"/>
+      <c r="BJ33"/>
+      <c r="BK33"/>
+      <c r="BL33"/>
+      <c r="BM33"/>
+      <c r="BN33"/>
+      <c r="BO33"/>
+      <c r="BP33"/>
+      <c r="BQ33"/>
+      <c r="BR33"/>
+      <c r="BS33"/>
+      <c r="BT33"/>
+      <c r="BU33"/>
+      <c r="BV33"/>
+      <c r="BW33"/>
+      <c r="BX33"/>
+      <c r="BY33"/>
+      <c r="BZ33"/>
+      <c r="CA33"/>
+      <c r="CB33"/>
+      <c r="CC33"/>
+      <c r="CD33"/>
+      <c r="CE33"/>
+      <c r="CF33"/>
+      <c r="CG33"/>
+      <c r="CH33"/>
+      <c r="CI33"/>
+      <c r="CJ33"/>
+      <c r="CK33"/>
+      <c r="CL33"/>
+      <c r="CM33"/>
+      <c r="CN33"/>
+      <c r="CO33"/>
+      <c r="CP33"/>
+      <c r="CQ33"/>
+      <c r="CR33"/>
+      <c r="CS33"/>
+      <c r="CT33"/>
+      <c r="CU33"/>
+      <c r="CV33"/>
+      <c r="CW33"/>
+      <c r="CX33"/>
+      <c r="CY33"/>
+      <c r="CZ33"/>
+      <c r="DA33"/>
+      <c r="DB33"/>
+      <c r="DC33"/>
+      <c r="DD33"/>
+      <c r="DE33"/>
+      <c r="DF33"/>
+      <c r="DG33"/>
+      <c r="DH33"/>
+      <c r="DI33"/>
+      <c r="DJ33"/>
+      <c r="DK33"/>
+      <c r="DL33"/>
+      <c r="DM33"/>
+      <c r="DN33"/>
+      <c r="DO33"/>
+      <c r="DP33"/>
+      <c r="DQ33"/>
+      <c r="DR33"/>
+      <c r="DS33"/>
+      <c r="DT33"/>
+      <c r="DU33"/>
+      <c r="DV33"/>
+      <c r="DW33"/>
+      <c r="DX33"/>
+      <c r="DY33"/>
+      <c r="DZ33"/>
+      <c r="EA33"/>
+      <c r="EB33"/>
+      <c r="EC33"/>
+      <c r="ED33"/>
+      <c r="EE33"/>
+      <c r="EF33"/>
+      <c r="EG33"/>
+      <c r="EH33"/>
+      <c r="EI33"/>
+      <c r="EJ33"/>
+      <c r="EK33"/>
+      <c r="EL33"/>
+      <c r="EM33"/>
+      <c r="EN33"/>
+      <c r="EO33"/>
+      <c r="EP33"/>
+      <c r="EQ33"/>
+      <c r="ER33"/>
+      <c r="ES33"/>
+      <c r="ET33"/>
+      <c r="EU33"/>
+      <c r="EV33"/>
+      <c r="EW33"/>
+      <c r="EX33"/>
+      <c r="EY33"/>
+      <c r="EZ33"/>
+      <c r="FA33"/>
+      <c r="FB33"/>
+      <c r="FC33"/>
+      <c r="FD33"/>
+      <c r="FE33"/>
+      <c r="FF33"/>
+      <c r="FG33"/>
+      <c r="FH33"/>
+      <c r="FI33"/>
+      <c r="FJ33"/>
+      <c r="FK33"/>
+      <c r="FL33"/>
+      <c r="FM33"/>
+      <c r="FN33"/>
+      <c r="FO33"/>
+      <c r="FP33"/>
+      <c r="FQ33"/>
+      <c r="FR33"/>
+      <c r="FS33"/>
+      <c r="FT33"/>
+      <c r="FU33"/>
+      <c r="FV33"/>
+      <c r="FW33"/>
+      <c r="FX33"/>
+      <c r="FY33"/>
+      <c r="FZ33"/>
+      <c r="GA33"/>
+      <c r="GB33"/>
+      <c r="GC33"/>
+      <c r="GD33"/>
+      <c r="GE33"/>
+      <c r="GF33"/>
+      <c r="GG33"/>
+      <c r="GH33"/>
+      <c r="GI33"/>
+      <c r="GJ33"/>
+      <c r="GK33"/>
+      <c r="GL33"/>
+      <c r="GM33"/>
+      <c r="GN33"/>
+      <c r="GO33"/>
+      <c r="GP33"/>
+      <c r="GQ33"/>
+      <c r="GR33"/>
+      <c r="GS33"/>
+      <c r="GT33"/>
+      <c r="GU33"/>
+      <c r="GV33"/>
+      <c r="GW33"/>
+      <c r="GX33"/>
+      <c r="GY33"/>
+      <c r="GZ33"/>
+      <c r="HA33"/>
+      <c r="HB33"/>
+      <c r="HC33"/>
+      <c r="HD33"/>
+      <c r="HE33"/>
+      <c r="HF33"/>
+      <c r="HG33"/>
+      <c r="HH33"/>
+      <c r="HI33"/>
+      <c r="HJ33"/>
+      <c r="HK33"/>
+      <c r="HL33"/>
+      <c r="HM33"/>
+      <c r="HN33"/>
+      <c r="HO33"/>
+      <c r="HP33"/>
+      <c r="HQ33"/>
+      <c r="HR33"/>
+      <c r="HS33"/>
+      <c r="HT33"/>
+      <c r="HU33"/>
+      <c r="HV33"/>
+      <c r="HW33"/>
+      <c r="HX33"/>
+      <c r="HY33"/>
+      <c r="HZ33"/>
+      <c r="IA33"/>
+      <c r="IB33"/>
+      <c r="IC33"/>
+      <c r="ID33"/>
+      <c r="IE33"/>
+      <c r="IF33"/>
+      <c r="IG33"/>
+      <c r="IH33"/>
+      <c r="II33"/>
+      <c r="IJ33"/>
+      <c r="IK33"/>
+      <c r="IL33"/>
+      <c r="IM33"/>
+      <c r="IN33"/>
+      <c r="IO33"/>
+      <c r="IP33"/>
+      <c r="IQ33"/>
+      <c r="IR33"/>
+      <c r="IS33"/>
+      <c r="IT33"/>
+      <c r="IU33"/>
+      <c r="IV33"/>
+      <c r="IW33"/>
+      <c r="IX33"/>
+      <c r="IY33"/>
+      <c r="IZ33"/>
+      <c r="JA33"/>
+      <c r="JB33"/>
+      <c r="JC33"/>
+      <c r="JD33"/>
+      <c r="JE33"/>
+      <c r="JF33"/>
+      <c r="JG33"/>
+      <c r="JH33"/>
+      <c r="JI33"/>
+      <c r="JJ33"/>
+      <c r="JK33"/>
+      <c r="JL33"/>
+      <c r="JM33"/>
+      <c r="JN33"/>
+      <c r="JO33"/>
+      <c r="JP33"/>
+      <c r="JQ33"/>
+      <c r="JR33"/>
+      <c r="JS33"/>
+      <c r="JT33"/>
+      <c r="JU33"/>
+      <c r="JV33"/>
+      <c r="JW33"/>
+      <c r="JX33"/>
+      <c r="JY33"/>
+      <c r="JZ33"/>
+      <c r="KA33"/>
+      <c r="KB33"/>
+      <c r="KC33"/>
+      <c r="KD33"/>
+      <c r="KE33"/>
+      <c r="KF33"/>
+      <c r="KG33"/>
+      <c r="KH33"/>
+      <c r="KI33"/>
+      <c r="KJ33"/>
+      <c r="KK33"/>
+      <c r="KL33"/>
+      <c r="KM33"/>
+      <c r="KN33"/>
+      <c r="KO33"/>
+      <c r="KP33"/>
+      <c r="KQ33"/>
+      <c r="KR33"/>
+      <c r="KS33"/>
+      <c r="KT33"/>
+      <c r="KU33"/>
+      <c r="KV33"/>
+      <c r="KW33"/>
+      <c r="KX33"/>
+      <c r="KY33"/>
+      <c r="KZ33"/>
+      <c r="LA33"/>
+      <c r="LB33"/>
+      <c r="LC33"/>
+      <c r="LD33"/>
+      <c r="LE33"/>
+      <c r="LF33"/>
+      <c r="LG33"/>
+      <c r="LH33"/>
+      <c r="LI33"/>
+      <c r="LJ33"/>
+      <c r="LK33"/>
+      <c r="LL33"/>
+      <c r="LM33"/>
+      <c r="LN33"/>
+      <c r="LO33"/>
+      <c r="LP33"/>
+      <c r="LQ33"/>
+      <c r="LR33"/>
+      <c r="LS33"/>
+      <c r="LT33"/>
+      <c r="LU33"/>
+      <c r="LV33"/>
+      <c r="LW33"/>
+      <c r="LX33"/>
+      <c r="LY33"/>
+      <c r="LZ33"/>
+      <c r="MA33"/>
+      <c r="MB33"/>
+      <c r="MC33"/>
+      <c r="MD33"/>
+      <c r="ME33"/>
+      <c r="MF33"/>
+      <c r="MG33"/>
+      <c r="MH33"/>
+      <c r="MI33"/>
+      <c r="MJ33"/>
+      <c r="MK33"/>
+      <c r="ML33"/>
+      <c r="MM33"/>
+      <c r="MN33"/>
+      <c r="MO33"/>
+      <c r="MP33"/>
+      <c r="MQ33"/>
+      <c r="MR33"/>
+      <c r="MS33"/>
+      <c r="MT33"/>
+      <c r="MU33"/>
+      <c r="MV33"/>
+      <c r="MW33"/>
+      <c r="MX33"/>
+      <c r="MY33"/>
+      <c r="MZ33"/>
+      <c r="NA33"/>
+      <c r="NB33"/>
+      <c r="NC33"/>
+      <c r="ND33"/>
+      <c r="NE33"/>
+      <c r="NF33"/>
+      <c r="NG33"/>
+      <c r="NH33"/>
+      <c r="NI33"/>
+      <c r="NJ33"/>
+      <c r="NK33"/>
+      <c r="NL33"/>
+      <c r="NM33"/>
+      <c r="NN33"/>
+      <c r="NO33"/>
+      <c r="NP33"/>
+      <c r="NQ33"/>
+      <c r="NR33"/>
+      <c r="NS33"/>
+      <c r="NT33"/>
+      <c r="NU33"/>
+      <c r="NV33"/>
+      <c r="NW33"/>
+      <c r="NX33"/>
+      <c r="NY33"/>
+      <c r="NZ33"/>
+      <c r="OA33"/>
+      <c r="OB33"/>
+      <c r="OC33"/>
+      <c r="OD33"/>
+      <c r="OE33"/>
+      <c r="OF33"/>
+      <c r="OG33"/>
+      <c r="OH33"/>
+      <c r="OI33"/>
+      <c r="OJ33"/>
+      <c r="OK33"/>
+      <c r="OL33"/>
+      <c r="OM33"/>
+      <c r="ON33"/>
+      <c r="OO33"/>
+      <c r="OP33"/>
+      <c r="OQ33"/>
+      <c r="OR33"/>
+      <c r="OS33"/>
+      <c r="OT33"/>
+      <c r="OU33"/>
+      <c r="OV33"/>
+      <c r="OW33"/>
+      <c r="OX33"/>
+      <c r="OY33"/>
+      <c r="OZ33"/>
+      <c r="PA33"/>
+      <c r="PB33"/>
+      <c r="PC33"/>
+      <c r="PD33"/>
+      <c r="PE33"/>
+      <c r="PF33"/>
+      <c r="PG33"/>
+      <c r="PH33"/>
+      <c r="PI33"/>
+      <c r="PJ33"/>
+      <c r="PK33"/>
+      <c r="PL33"/>
+      <c r="PM33"/>
+      <c r="PN33"/>
+      <c r="PO33"/>
+      <c r="PP33"/>
+      <c r="PQ33"/>
+      <c r="PR33"/>
+      <c r="PS33"/>
+      <c r="PT33"/>
+      <c r="PU33"/>
+      <c r="PV33"/>
+      <c r="PW33"/>
+      <c r="PX33"/>
+      <c r="PY33"/>
+      <c r="PZ33"/>
+      <c r="QA33"/>
+      <c r="QB33"/>
+      <c r="QC33"/>
+      <c r="QD33"/>
+      <c r="QE33"/>
+      <c r="QF33"/>
+      <c r="QG33"/>
+      <c r="QH33"/>
+      <c r="QI33"/>
+      <c r="QJ33"/>
+      <c r="QK33"/>
+      <c r="QL33"/>
+      <c r="QM33"/>
+      <c r="QN33"/>
+      <c r="QO33"/>
+      <c r="QP33"/>
+      <c r="QQ33"/>
+      <c r="QR33"/>
+      <c r="QS33"/>
+      <c r="QT33"/>
+      <c r="QU33"/>
+      <c r="QV33"/>
+      <c r="QW33"/>
+      <c r="QX33"/>
+      <c r="QY33"/>
+      <c r="QZ33"/>
+      <c r="RA33"/>
+      <c r="RB33"/>
+      <c r="RC33"/>
+      <c r="RD33"/>
+      <c r="RE33"/>
+      <c r="RF33"/>
+      <c r="RG33"/>
+      <c r="RH33"/>
+      <c r="RI33"/>
+      <c r="RJ33"/>
+      <c r="RK33"/>
+      <c r="RL33"/>
+      <c r="RM33"/>
+      <c r="RN33"/>
+    </row>
+    <row r="34" spans="1:482" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L34" s="7"/>
+      <c r="M34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD34"/>
+      <c r="AE34"/>
+      <c r="AF34"/>
+      <c r="AG34"/>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AJ34"/>
+      <c r="AK34"/>
+      <c r="AL34"/>
+      <c r="AM34"/>
+      <c r="AN34"/>
+      <c r="AO34"/>
+      <c r="AP34"/>
+      <c r="AQ34"/>
+      <c r="AR34"/>
+      <c r="AS34"/>
+      <c r="AT34"/>
+      <c r="AU34"/>
+      <c r="AV34"/>
+      <c r="AW34"/>
+      <c r="AX34"/>
+      <c r="AY34"/>
+      <c r="AZ34"/>
+      <c r="BA34"/>
+      <c r="BB34"/>
+      <c r="BC34"/>
+      <c r="BD34"/>
+      <c r="BE34"/>
+      <c r="BF34"/>
+      <c r="BG34"/>
+      <c r="BH34"/>
+      <c r="BI34"/>
+      <c r="BJ34"/>
+      <c r="BK34"/>
+      <c r="BL34"/>
+      <c r="BM34"/>
+      <c r="BN34"/>
+      <c r="BO34"/>
+      <c r="BP34"/>
+      <c r="BQ34"/>
+      <c r="BR34"/>
+      <c r="BS34"/>
+      <c r="BT34"/>
+      <c r="BU34"/>
+      <c r="BV34"/>
+      <c r="BW34"/>
+      <c r="BX34"/>
+      <c r="BY34"/>
+      <c r="BZ34"/>
+      <c r="CA34"/>
+      <c r="CB34"/>
+      <c r="CC34"/>
+      <c r="CD34"/>
+      <c r="CE34"/>
+      <c r="CF34"/>
+      <c r="CG34"/>
+      <c r="CH34"/>
+      <c r="CI34"/>
+      <c r="CJ34"/>
+      <c r="CK34"/>
+      <c r="CL34"/>
+      <c r="CM34"/>
+      <c r="CN34"/>
+      <c r="CO34"/>
+      <c r="CP34"/>
+      <c r="CQ34"/>
+      <c r="CR34"/>
+      <c r="CS34"/>
+      <c r="CT34"/>
+      <c r="CU34"/>
+      <c r="CV34"/>
+      <c r="CW34"/>
+      <c r="CX34"/>
+      <c r="CY34"/>
+      <c r="CZ34"/>
+      <c r="DA34"/>
+      <c r="DB34"/>
+      <c r="DC34"/>
+      <c r="DD34"/>
+      <c r="DE34"/>
+      <c r="DF34"/>
+      <c r="DG34"/>
+      <c r="DH34"/>
+      <c r="DI34"/>
+      <c r="DJ34"/>
+      <c r="DK34"/>
+      <c r="DL34"/>
+      <c r="DM34"/>
+      <c r="DN34"/>
+      <c r="DO34"/>
+      <c r="DP34"/>
+      <c r="DQ34"/>
+      <c r="DR34"/>
+      <c r="DS34"/>
+      <c r="DT34"/>
+      <c r="DU34"/>
+      <c r="DV34"/>
+      <c r="DW34"/>
+      <c r="DX34"/>
+      <c r="DY34"/>
+      <c r="DZ34"/>
+      <c r="EA34"/>
+      <c r="EB34"/>
+      <c r="EC34"/>
+      <c r="ED34"/>
+      <c r="EE34"/>
+      <c r="EF34"/>
+      <c r="EG34"/>
+      <c r="EH34"/>
+      <c r="EI34"/>
+      <c r="EJ34"/>
+      <c r="EK34"/>
+      <c r="EL34"/>
+      <c r="EM34"/>
+      <c r="EN34"/>
+      <c r="EO34"/>
+      <c r="EP34"/>
+      <c r="EQ34"/>
+      <c r="ER34"/>
+      <c r="ES34"/>
+      <c r="ET34"/>
+      <c r="EU34"/>
+      <c r="EV34"/>
+      <c r="EW34"/>
+      <c r="EX34"/>
+      <c r="EY34"/>
+      <c r="EZ34"/>
+      <c r="FA34"/>
+      <c r="FB34"/>
+      <c r="FC34"/>
+      <c r="FD34"/>
+      <c r="FE34"/>
+      <c r="FF34"/>
+      <c r="FG34"/>
+      <c r="FH34"/>
+      <c r="FI34"/>
+      <c r="FJ34"/>
+      <c r="FK34"/>
+      <c r="FL34"/>
+      <c r="FM34"/>
+      <c r="FN34"/>
+      <c r="FO34"/>
+      <c r="FP34"/>
+      <c r="FQ34"/>
+      <c r="FR34"/>
+      <c r="FS34"/>
+      <c r="FT34"/>
+      <c r="FU34"/>
+      <c r="FV34"/>
+      <c r="FW34"/>
+      <c r="FX34"/>
+      <c r="FY34"/>
+      <c r="FZ34"/>
+      <c r="GA34"/>
+      <c r="GB34"/>
+      <c r="GC34"/>
+      <c r="GD34"/>
+      <c r="GE34"/>
+      <c r="GF34"/>
+      <c r="GG34"/>
+      <c r="GH34"/>
+      <c r="GI34"/>
+      <c r="GJ34"/>
+      <c r="GK34"/>
+      <c r="GL34"/>
+      <c r="GM34"/>
+      <c r="GN34"/>
+      <c r="GO34"/>
+      <c r="GP34"/>
+      <c r="GQ34"/>
+      <c r="GR34"/>
+      <c r="GS34"/>
+      <c r="GT34"/>
+      <c r="GU34"/>
+      <c r="GV34"/>
+      <c r="GW34"/>
+      <c r="GX34"/>
+      <c r="GY34"/>
+      <c r="GZ34"/>
+      <c r="HA34"/>
+      <c r="HB34"/>
+      <c r="HC34"/>
+      <c r="HD34"/>
+      <c r="HE34"/>
+      <c r="HF34"/>
+      <c r="HG34"/>
+      <c r="HH34"/>
+      <c r="HI34"/>
+      <c r="HJ34"/>
+      <c r="HK34"/>
+      <c r="HL34"/>
+      <c r="HM34"/>
+      <c r="HN34"/>
+      <c r="HO34"/>
+      <c r="HP34"/>
+      <c r="HQ34"/>
+      <c r="HR34"/>
+      <c r="HS34"/>
+      <c r="HT34"/>
+      <c r="HU34"/>
+      <c r="HV34"/>
+      <c r="HW34"/>
+      <c r="HX34"/>
+      <c r="HY34"/>
+      <c r="HZ34"/>
+      <c r="IA34"/>
+      <c r="IB34"/>
+      <c r="IC34"/>
+      <c r="ID34"/>
+      <c r="IE34"/>
+      <c r="IF34"/>
+      <c r="IG34"/>
+      <c r="IH34"/>
+      <c r="II34"/>
+      <c r="IJ34"/>
+      <c r="IK34"/>
+      <c r="IL34"/>
+      <c r="IM34"/>
+      <c r="IN34"/>
+      <c r="IO34"/>
+      <c r="IP34"/>
+      <c r="IQ34"/>
+      <c r="IR34"/>
+      <c r="IS34"/>
+      <c r="IT34"/>
+      <c r="IU34"/>
+      <c r="IV34"/>
+      <c r="IW34"/>
+      <c r="IX34"/>
+      <c r="IY34"/>
+      <c r="IZ34"/>
+      <c r="JA34"/>
+      <c r="JB34"/>
+      <c r="JC34"/>
+      <c r="JD34"/>
+      <c r="JE34"/>
+      <c r="JF34"/>
+      <c r="JG34"/>
+      <c r="JH34"/>
+      <c r="JI34"/>
+      <c r="JJ34"/>
+      <c r="JK34"/>
+      <c r="JL34"/>
+      <c r="JM34"/>
+      <c r="JN34"/>
+      <c r="JO34"/>
+      <c r="JP34"/>
+      <c r="JQ34"/>
+      <c r="JR34"/>
+      <c r="JS34"/>
+      <c r="JT34"/>
+      <c r="JU34"/>
+      <c r="JV34"/>
+      <c r="JW34"/>
+      <c r="JX34"/>
+      <c r="JY34"/>
+      <c r="JZ34"/>
+      <c r="KA34"/>
+      <c r="KB34"/>
+      <c r="KC34"/>
+      <c r="KD34"/>
+      <c r="KE34"/>
+      <c r="KF34"/>
+      <c r="KG34"/>
+      <c r="KH34"/>
+      <c r="KI34"/>
+      <c r="KJ34"/>
+      <c r="KK34"/>
+      <c r="KL34"/>
+      <c r="KM34"/>
+      <c r="KN34"/>
+      <c r="KO34"/>
+      <c r="KP34"/>
+      <c r="KQ34"/>
+      <c r="KR34"/>
+      <c r="KS34"/>
+      <c r="KT34"/>
+      <c r="KU34"/>
+      <c r="KV34"/>
+      <c r="KW34"/>
+      <c r="KX34"/>
+      <c r="KY34"/>
+      <c r="KZ34"/>
+      <c r="LA34"/>
+      <c r="LB34"/>
+      <c r="LC34"/>
+      <c r="LD34"/>
+      <c r="LE34"/>
+      <c r="LF34"/>
+      <c r="LG34"/>
+      <c r="LH34"/>
+      <c r="LI34"/>
+      <c r="LJ34"/>
+      <c r="LK34"/>
+      <c r="LL34"/>
+      <c r="LM34"/>
+      <c r="LN34"/>
+      <c r="LO34"/>
+      <c r="LP34"/>
+      <c r="LQ34"/>
+      <c r="LR34"/>
+      <c r="LS34"/>
+      <c r="LT34"/>
+      <c r="LU34"/>
+      <c r="LV34"/>
+      <c r="LW34"/>
+      <c r="LX34"/>
+      <c r="LY34"/>
+      <c r="LZ34"/>
+      <c r="MA34"/>
+      <c r="MB34"/>
+      <c r="MC34"/>
+      <c r="MD34"/>
+      <c r="ME34"/>
+      <c r="MF34"/>
+      <c r="MG34"/>
+      <c r="MH34"/>
+      <c r="MI34"/>
+      <c r="MJ34"/>
+      <c r="MK34"/>
+      <c r="ML34"/>
+      <c r="MM34"/>
+      <c r="MN34"/>
+      <c r="MO34"/>
+      <c r="MP34"/>
+      <c r="MQ34"/>
+      <c r="MR34"/>
+      <c r="MS34"/>
+      <c r="MT34"/>
+      <c r="MU34"/>
+      <c r="MV34"/>
+      <c r="MW34"/>
+      <c r="MX34"/>
+      <c r="MY34"/>
+      <c r="MZ34"/>
+      <c r="NA34"/>
+      <c r="NB34"/>
+      <c r="NC34"/>
+      <c r="ND34"/>
+      <c r="NE34"/>
+      <c r="NF34"/>
+      <c r="NG34"/>
+      <c r="NH34"/>
+      <c r="NI34"/>
+      <c r="NJ34"/>
+      <c r="NK34"/>
+      <c r="NL34"/>
+      <c r="NM34"/>
+      <c r="NN34"/>
+      <c r="NO34"/>
+      <c r="NP34"/>
+      <c r="NQ34"/>
+      <c r="NR34"/>
+      <c r="NS34"/>
+      <c r="NT34"/>
+      <c r="NU34"/>
+      <c r="NV34"/>
+      <c r="NW34"/>
+      <c r="NX34"/>
+      <c r="NY34"/>
+      <c r="NZ34"/>
+      <c r="OA34"/>
+      <c r="OB34"/>
+      <c r="OC34"/>
+      <c r="OD34"/>
+      <c r="OE34"/>
+      <c r="OF34"/>
+      <c r="OG34"/>
+      <c r="OH34"/>
+      <c r="OI34"/>
+      <c r="OJ34"/>
+      <c r="OK34"/>
+      <c r="OL34"/>
+      <c r="OM34"/>
+      <c r="ON34"/>
+      <c r="OO34"/>
+      <c r="OP34"/>
+      <c r="OQ34"/>
+      <c r="OR34"/>
+      <c r="OS34"/>
+      <c r="OT34"/>
+      <c r="OU34"/>
+      <c r="OV34"/>
+      <c r="OW34"/>
+      <c r="OX34"/>
+      <c r="OY34"/>
+      <c r="OZ34"/>
+      <c r="PA34"/>
+      <c r="PB34"/>
+      <c r="PC34"/>
+      <c r="PD34"/>
+      <c r="PE34"/>
+      <c r="PF34"/>
+      <c r="PG34"/>
+      <c r="PH34"/>
+      <c r="PI34"/>
+      <c r="PJ34"/>
+      <c r="PK34"/>
+      <c r="PL34"/>
+      <c r="PM34"/>
+      <c r="PN34"/>
+      <c r="PO34"/>
+      <c r="PP34"/>
+      <c r="PQ34"/>
+      <c r="PR34"/>
+      <c r="PS34"/>
+      <c r="PT34"/>
+      <c r="PU34"/>
+      <c r="PV34"/>
+      <c r="PW34"/>
+      <c r="PX34"/>
+      <c r="PY34"/>
+      <c r="PZ34"/>
+      <c r="QA34"/>
+      <c r="QB34"/>
+      <c r="QC34"/>
+      <c r="QD34"/>
+      <c r="QE34"/>
+      <c r="QF34"/>
+      <c r="QG34"/>
+      <c r="QH34"/>
+      <c r="QI34"/>
+      <c r="QJ34"/>
+      <c r="QK34"/>
+      <c r="QL34"/>
+      <c r="QM34"/>
+      <c r="QN34"/>
+      <c r="QO34"/>
+      <c r="QP34"/>
+      <c r="QQ34"/>
+      <c r="QR34"/>
+      <c r="QS34"/>
+      <c r="QT34"/>
+      <c r="QU34"/>
+      <c r="QV34"/>
+      <c r="QW34"/>
+      <c r="QX34"/>
+      <c r="QY34"/>
+      <c r="QZ34"/>
+      <c r="RA34"/>
+      <c r="RB34"/>
+      <c r="RC34"/>
+      <c r="RD34"/>
+      <c r="RE34"/>
+      <c r="RF34"/>
+      <c r="RG34"/>
+      <c r="RH34"/>
+      <c r="RI34"/>
+      <c r="RJ34"/>
+      <c r="RK34"/>
+      <c r="RL34"/>
+      <c r="RM34"/>
+      <c r="RN34"/>
+    </row>
+    <row r="35" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+      <c r="V35" s="15"/>
+      <c r="W35" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="X35" s="15"/>
+      <c r="Y35" s="15"/>
+      <c r="Z35" s="15"/>
+      <c r="AA35" s="15"/>
+      <c r="AB35" s="15"/>
+      <c r="AC35" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+      <c r="AR35"/>
+      <c r="AS35"/>
+      <c r="AT35"/>
+      <c r="AU35"/>
+      <c r="AV35"/>
+      <c r="AW35"/>
+      <c r="AX35"/>
+      <c r="AY35"/>
+      <c r="AZ35"/>
+      <c r="BA35"/>
+      <c r="BB35"/>
+      <c r="BC35"/>
+      <c r="BD35"/>
+      <c r="BE35"/>
+      <c r="BF35"/>
+      <c r="BG35"/>
+      <c r="BH35"/>
+      <c r="BI35"/>
+      <c r="BJ35"/>
+      <c r="BK35"/>
+      <c r="BL35"/>
+      <c r="BM35"/>
+      <c r="BN35"/>
+      <c r="BO35"/>
+      <c r="BP35"/>
+      <c r="BQ35"/>
+      <c r="BR35"/>
+      <c r="BS35"/>
+      <c r="BT35"/>
+      <c r="BU35"/>
+      <c r="BV35"/>
+      <c r="BW35"/>
+      <c r="BX35"/>
+      <c r="BY35"/>
+      <c r="BZ35"/>
+      <c r="CA35"/>
+      <c r="CB35"/>
+      <c r="CC35"/>
+      <c r="CD35"/>
+      <c r="CE35"/>
+      <c r="CF35"/>
+      <c r="CG35"/>
+      <c r="CH35"/>
+      <c r="CI35"/>
+      <c r="CJ35"/>
+      <c r="CK35"/>
+      <c r="CL35"/>
+      <c r="CM35"/>
+      <c r="CN35"/>
+      <c r="CO35"/>
+      <c r="CP35"/>
+      <c r="CQ35"/>
+      <c r="CR35"/>
+      <c r="CS35"/>
+      <c r="CT35"/>
+      <c r="CU35"/>
+      <c r="CV35"/>
+      <c r="CW35"/>
+      <c r="CX35"/>
+      <c r="CY35"/>
+      <c r="CZ35"/>
+      <c r="DA35"/>
+      <c r="DB35"/>
+      <c r="DC35"/>
+      <c r="DD35"/>
+      <c r="DE35"/>
+      <c r="DF35"/>
+      <c r="DG35"/>
+      <c r="DH35"/>
+      <c r="DI35"/>
+      <c r="DJ35"/>
+      <c r="DK35"/>
+      <c r="DL35"/>
+      <c r="DM35"/>
+      <c r="DN35"/>
+      <c r="DO35"/>
+      <c r="DP35"/>
+      <c r="DQ35"/>
+      <c r="DR35"/>
+      <c r="DS35"/>
+      <c r="DT35"/>
+      <c r="DU35"/>
+      <c r="DV35"/>
+      <c r="DW35"/>
+      <c r="DX35"/>
+      <c r="DY35"/>
+      <c r="DZ35"/>
+      <c r="EA35"/>
+      <c r="EB35"/>
+      <c r="EC35"/>
+      <c r="ED35"/>
+      <c r="EE35"/>
+      <c r="EF35"/>
+      <c r="EG35"/>
+      <c r="EH35"/>
+      <c r="EI35"/>
+      <c r="EJ35"/>
+      <c r="EK35"/>
+      <c r="EL35"/>
+      <c r="EM35"/>
+      <c r="EN35"/>
+      <c r="EO35"/>
+      <c r="EP35"/>
+      <c r="EQ35"/>
+      <c r="ER35"/>
+      <c r="ES35"/>
+      <c r="ET35"/>
+      <c r="EU35"/>
+      <c r="EV35"/>
+      <c r="EW35"/>
+      <c r="EX35"/>
+      <c r="EY35"/>
+      <c r="EZ35"/>
+      <c r="FA35"/>
+      <c r="FB35"/>
+      <c r="FC35"/>
+      <c r="FD35"/>
+      <c r="FE35"/>
+      <c r="FF35"/>
+      <c r="FG35"/>
+      <c r="FH35"/>
+      <c r="FI35"/>
+      <c r="FJ35"/>
+      <c r="FK35"/>
+      <c r="FL35"/>
+      <c r="FM35"/>
+      <c r="FN35"/>
+      <c r="FO35"/>
+      <c r="FP35"/>
+      <c r="FQ35"/>
+      <c r="FR35"/>
+      <c r="FS35"/>
+      <c r="FT35"/>
+      <c r="FU35"/>
+      <c r="FV35"/>
+      <c r="FW35"/>
+      <c r="FX35"/>
+      <c r="FY35"/>
+      <c r="FZ35"/>
+      <c r="GA35"/>
+      <c r="GB35"/>
+      <c r="GC35"/>
+      <c r="GD35"/>
+      <c r="GE35"/>
+      <c r="GF35"/>
+      <c r="GG35"/>
+      <c r="GH35"/>
+      <c r="GI35"/>
+      <c r="GJ35"/>
+      <c r="GK35"/>
+      <c r="GL35"/>
+      <c r="GM35"/>
+      <c r="GN35"/>
+      <c r="GO35"/>
+      <c r="GP35"/>
+      <c r="GQ35"/>
+      <c r="GR35"/>
+      <c r="GS35"/>
+      <c r="GT35"/>
+      <c r="GU35"/>
+      <c r="GV35"/>
+      <c r="GW35"/>
+      <c r="GX35"/>
+      <c r="GY35"/>
+      <c r="GZ35"/>
+      <c r="HA35"/>
+      <c r="HB35"/>
+      <c r="HC35"/>
+      <c r="HD35"/>
+      <c r="HE35"/>
+      <c r="HF35"/>
+      <c r="HG35"/>
+      <c r="HH35"/>
+      <c r="HI35"/>
+      <c r="HJ35"/>
+      <c r="HK35"/>
+      <c r="HL35"/>
+      <c r="HM35"/>
+      <c r="HN35"/>
+      <c r="HO35"/>
+      <c r="HP35"/>
+      <c r="HQ35"/>
+      <c r="HR35"/>
+      <c r="HS35"/>
+      <c r="HT35"/>
+      <c r="HU35"/>
+      <c r="HV35"/>
+      <c r="HW35"/>
+      <c r="HX35"/>
+      <c r="HY35"/>
+      <c r="HZ35"/>
+      <c r="IA35"/>
+      <c r="IB35"/>
+      <c r="IC35"/>
+      <c r="ID35"/>
+      <c r="IE35"/>
+      <c r="IF35"/>
+      <c r="IG35"/>
+      <c r="IH35"/>
+      <c r="II35"/>
+      <c r="IJ35"/>
+      <c r="IK35"/>
+      <c r="IL35"/>
+      <c r="IM35"/>
+      <c r="IN35"/>
+      <c r="IO35"/>
+      <c r="IP35"/>
+      <c r="IQ35"/>
+      <c r="IR35"/>
+      <c r="IS35"/>
+      <c r="IT35"/>
+      <c r="IU35"/>
+      <c r="IV35"/>
+      <c r="IW35"/>
+      <c r="IX35"/>
+      <c r="IY35"/>
+      <c r="IZ35"/>
+      <c r="JA35"/>
+      <c r="JB35"/>
+      <c r="JC35"/>
+      <c r="JD35"/>
+      <c r="JE35"/>
+      <c r="JF35"/>
+      <c r="JG35"/>
+      <c r="JH35"/>
+      <c r="JI35"/>
+      <c r="JJ35"/>
+      <c r="JK35"/>
+      <c r="JL35"/>
+      <c r="JM35"/>
+      <c r="JN35"/>
+      <c r="JO35"/>
+      <c r="JP35"/>
+      <c r="JQ35"/>
+      <c r="JR35"/>
+      <c r="JS35"/>
+      <c r="JT35"/>
+      <c r="JU35"/>
+      <c r="JV35"/>
+      <c r="JW35"/>
+      <c r="JX35"/>
+      <c r="JY35"/>
+      <c r="JZ35"/>
+      <c r="KA35"/>
+      <c r="KB35"/>
+      <c r="KC35"/>
+      <c r="KD35"/>
+      <c r="KE35"/>
+      <c r="KF35"/>
+      <c r="KG35"/>
+      <c r="KH35"/>
+      <c r="KI35"/>
+      <c r="KJ35"/>
+      <c r="KK35"/>
+      <c r="KL35"/>
+      <c r="KM35"/>
+      <c r="KN35"/>
+      <c r="KO35"/>
+      <c r="KP35"/>
+      <c r="KQ35"/>
+      <c r="KR35"/>
+      <c r="KS35"/>
+      <c r="KT35"/>
+      <c r="KU35"/>
+      <c r="KV35"/>
+      <c r="KW35"/>
+      <c r="KX35"/>
+      <c r="KY35"/>
+      <c r="KZ35"/>
+      <c r="LA35"/>
+      <c r="LB35"/>
+      <c r="LC35"/>
+      <c r="LD35"/>
+      <c r="LE35"/>
+      <c r="LF35"/>
+      <c r="LG35"/>
+      <c r="LH35"/>
+      <c r="LI35"/>
+      <c r="LJ35"/>
+      <c r="LK35"/>
+      <c r="LL35"/>
+      <c r="LM35"/>
+      <c r="LN35"/>
+      <c r="LO35"/>
+      <c r="LP35"/>
+      <c r="LQ35"/>
+      <c r="LR35"/>
+      <c r="LS35"/>
+      <c r="LT35"/>
+      <c r="LU35"/>
+      <c r="LV35"/>
+      <c r="LW35"/>
+      <c r="LX35"/>
+      <c r="LY35"/>
+      <c r="LZ35"/>
+      <c r="MA35"/>
+      <c r="MB35"/>
+      <c r="MC35"/>
+      <c r="MD35"/>
+      <c r="ME35"/>
+      <c r="MF35"/>
+      <c r="MG35"/>
+      <c r="MH35"/>
+      <c r="MI35"/>
+      <c r="MJ35"/>
+      <c r="MK35"/>
+      <c r="ML35"/>
+      <c r="MM35"/>
+      <c r="MN35"/>
+      <c r="MO35"/>
+      <c r="MP35"/>
+      <c r="MQ35"/>
+      <c r="MR35"/>
+      <c r="MS35"/>
+      <c r="MT35"/>
+      <c r="MU35"/>
+      <c r="MV35"/>
+      <c r="MW35"/>
+      <c r="MX35"/>
+      <c r="MY35"/>
+      <c r="MZ35"/>
+      <c r="NA35"/>
+      <c r="NB35"/>
+      <c r="NC35"/>
+      <c r="ND35"/>
+      <c r="NE35"/>
+      <c r="NF35"/>
+      <c r="NG35"/>
+      <c r="NH35"/>
+      <c r="NI35"/>
+      <c r="NJ35"/>
+      <c r="NK35"/>
+      <c r="NL35"/>
+      <c r="NM35"/>
+      <c r="NN35"/>
+      <c r="NO35"/>
+      <c r="NP35"/>
+      <c r="NQ35"/>
+      <c r="NR35"/>
+      <c r="NS35"/>
+      <c r="NT35"/>
+      <c r="NU35"/>
+      <c r="NV35"/>
+      <c r="NW35"/>
+      <c r="NX35"/>
+      <c r="NY35"/>
+      <c r="NZ35"/>
+      <c r="OA35"/>
+      <c r="OB35"/>
+      <c r="OC35"/>
+      <c r="OD35"/>
+      <c r="OE35"/>
+      <c r="OF35"/>
+      <c r="OG35"/>
+      <c r="OH35"/>
+      <c r="OI35"/>
+      <c r="OJ35"/>
+      <c r="OK35"/>
+      <c r="OL35"/>
+      <c r="OM35"/>
+      <c r="ON35"/>
+      <c r="OO35"/>
+      <c r="OP35"/>
+      <c r="OQ35"/>
+      <c r="OR35"/>
+      <c r="OS35"/>
+      <c r="OT35"/>
+      <c r="OU35"/>
+      <c r="OV35"/>
+      <c r="OW35"/>
+      <c r="OX35"/>
+      <c r="OY35"/>
+      <c r="OZ35"/>
+      <c r="PA35"/>
+      <c r="PB35"/>
+      <c r="PC35"/>
+      <c r="PD35"/>
+      <c r="PE35"/>
+      <c r="PF35"/>
+      <c r="PG35"/>
+      <c r="PH35"/>
+      <c r="PI35"/>
+      <c r="PJ35"/>
+      <c r="PK35"/>
+      <c r="PL35"/>
+      <c r="PM35"/>
+      <c r="PN35"/>
+      <c r="PO35"/>
+      <c r="PP35"/>
+      <c r="PQ35"/>
+      <c r="PR35"/>
+      <c r="PS35"/>
+      <c r="PT35"/>
+      <c r="PU35"/>
+      <c r="PV35"/>
+      <c r="PW35"/>
+      <c r="PX35"/>
+      <c r="PY35"/>
+      <c r="PZ35"/>
+      <c r="QA35"/>
+      <c r="QB35"/>
+      <c r="QC35"/>
+      <c r="QD35"/>
+      <c r="QE35"/>
+      <c r="QF35"/>
+      <c r="QG35"/>
+      <c r="QH35"/>
+      <c r="QI35"/>
+      <c r="QJ35"/>
+      <c r="QK35"/>
+      <c r="QL35"/>
+      <c r="QM35"/>
+      <c r="QN35"/>
+      <c r="QO35"/>
+      <c r="QP35"/>
+      <c r="QQ35"/>
+      <c r="QR35"/>
+      <c r="QS35"/>
+      <c r="QT35"/>
+      <c r="QU35"/>
+      <c r="QV35"/>
+      <c r="QW35"/>
+      <c r="QX35"/>
+      <c r="QY35"/>
+      <c r="QZ35"/>
+      <c r="RA35"/>
+      <c r="RB35"/>
+      <c r="RC35"/>
+      <c r="RD35"/>
+      <c r="RE35"/>
+      <c r="RF35"/>
+      <c r="RG35"/>
+      <c r="RH35"/>
+      <c r="RI35"/>
+      <c r="RJ35"/>
+      <c r="RK35"/>
+      <c r="RL35"/>
+      <c r="RM35"/>
+      <c r="RN35"/>
+    </row>
+    <row r="36" spans="1:482" ht="34" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:482" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:482" x14ac:dyDescent="0.2">
+      <c r="AD38" t="s">
         <v>114</v>
       </c>
-      <c r="D33" t="s">
-        <v>111</v>
-      </c>
     </row>
-    <row r="34" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" t="s">
-        <v>112</v>
-      </c>
+    <row r="43" spans="1:482" x14ac:dyDescent="0.2">
+      <c r="C43" s="5"/>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="AD35" t="s">
-        <v>116</v>
-      </c>
+    <row r="45" spans="1:482" x14ac:dyDescent="0.2">
+      <c r="C45" s="5"/>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="C40" s="5"/>
-    </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="C42" s="5"/>
-    </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="C44" s="5"/>
+    <row r="47" spans="1:482" x14ac:dyDescent="0.2">
+      <c r="C47" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix(excel2xml): proper handling of special characters in text properties, depending on the encoding (DEV-1719) (#296)
</commit_message>
<xml_diff>
--- a/testdata/excel2xml-testdata.xlsx
+++ b/testdata/excel2xml-testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52D4EAF-34A2-174B-B0AE-B44196716646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A49BD9-00EA-8D40-8CB4-6080470F3D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{8DC9C588-8EAF-9149-8D6F-E65826635888}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20500" xr2:uid="{8DC9C588-8EAF-9149-8D6F-E65826635888}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="141">
   <si>
     <t>id</t>
   </si>
@@ -713,9 +713,6 @@
     <t>Iliad Prooem</t>
   </si>
   <si>
-    <t>This page shows the prooem of the Iliad in Greek manuscript 1397 in St. Catherine's Monastery on Mount Sinai.</t>
-  </si>
-  <si>
     <t>:hasCopyright</t>
   </si>
   <si>
@@ -904,6 +901,12 @@
   </si>
   <si>
     <t>:hasFourthLink</t>
+  </si>
+  <si>
+    <t>Iliad Prooem ' and a single quote in utf8</t>
+  </si>
+  <si>
+    <t>Iliad Prooem ' and a single quote in xml</t>
   </si>
 </sst>
 </file>
@@ -1437,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B59957-CA62-894B-8744-01ADFD605729}">
   <dimension ref="A1:RN47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1881,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -1893,7 +1896,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>6</v>
@@ -1953,7 +1956,7 @@
         <v>24</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD1"/>
       <c r="AE1"/>
@@ -1961,7 +1964,7 @@
       <c r="AG1"/>
       <c r="AH1"/>
       <c r="AI1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ1"/>
       <c r="AK1"/>
@@ -2422,7 +2425,7 @@
         <v>48</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>25</v>
@@ -2435,7 +2438,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2"/>
       <c r="AD2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AE2"/>
       <c r="AF2"/>
@@ -2920,7 +2923,7 @@
       </c>
       <c r="T3" s="7"/>
       <c r="U3" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V3" s="6" t="s">
         <v>28</v>
@@ -2930,7 +2933,7 @@
       </c>
       <c r="X3" s="7"/>
       <c r="Y3" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Z3" s="6" t="s">
         <v>28</v>
@@ -2942,7 +2945,7 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AF3"/>
       <c r="AG3"/>
@@ -3406,28 +3409,28 @@
       </c>
       <c r="L4" s="7"/>
       <c r="M4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T4" s="7"/>
       <c r="U4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="W4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="X4" s="7"/>
       <c r="Y4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AA4" s="6" t="s">
         <v>29</v>
@@ -3898,28 +3901,28 @@
       </c>
       <c r="L5" s="7"/>
       <c r="M5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="W5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="X5" s="7"/>
       <c r="Y5" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AA5" s="6" t="s">
         <v>29</v>
@@ -4383,35 +4386,35 @@
     <row r="6" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I6" s="7"/>
       <c r="J6" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>51</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P6" s="7"/>
       <c r="Q6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="X6" s="7"/>
       <c r="Y6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA6" s="6" t="s">
         <v>29</v>
@@ -4875,35 +4878,35 @@
     <row r="7" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I7" s="7"/>
       <c r="J7" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>51</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="P7" s="7"/>
       <c r="Q7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="X7" s="7"/>
       <c r="Y7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AA7" s="6" t="s">
         <v>29</v>
@@ -5375,14 +5378,14 @@
       <c r="H8" s="10"/>
       <c r="I8" s="11"/>
       <c r="J8" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>51</v>
       </c>
       <c r="L8" s="11"/>
       <c r="M8" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
@@ -5877,12 +5880,12 @@
       <c r="AB9" s="7"/>
       <c r="AC9"/>
       <c r="AD9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AE9"/>
       <c r="AF9"/>
       <c r="AG9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AH9"/>
       <c r="AI9"/>
@@ -7307,7 +7310,7 @@
         <v>25</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>29</v>
@@ -7796,7 +7799,7 @@
       </c>
       <c r="L13" s="7"/>
       <c r="M13" s="17" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>28</v>
@@ -7812,7 +7815,7 @@
       <c r="Y13" s="17"/>
       <c r="AB13" s="7"/>
       <c r="AC13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD13"/>
       <c r="AE13"/>
@@ -8278,7 +8281,7 @@
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="17" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="N14" s="6" t="s">
         <v>31</v>
@@ -8751,14 +8754,14 @@
     <row r="15" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I15" s="7"/>
       <c r="J15" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>27</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>31</v>
@@ -9232,16 +9235,16 @@
       <c r="H16" s="10"/>
       <c r="I16" s="11"/>
       <c r="J16" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>32</v>
       </c>
       <c r="L16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="M16" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10" t="s">
@@ -9723,10 +9726,10 @@
         <v>38</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -10220,7 +10223,7 @@
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>28</v>
@@ -11181,20 +11184,20 @@
     </row>
     <row r="20" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>91</v>
-      </c>
       <c r="E20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F20"/>
       <c r="G20" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I20" s="7"/>
       <c r="L20" s="7"/>
@@ -11667,7 +11670,7 @@
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N21" s="6" t="s">
         <v>28</v>
@@ -12146,14 +12149,14 @@
     <row r="22" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I22" s="7"/>
       <c r="J22" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O22" s="6" t="s">
         <v>61</v>
@@ -12620,14 +12623,14 @@
     <row r="23" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I23" s="7"/>
       <c r="J23" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L23" s="7"/>
       <c r="M23" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O23" s="6" t="s">
         <v>61</v>
@@ -13097,7 +13100,7 @@
       <c r="G24" s="10"/>
       <c r="I24" s="11"/>
       <c r="J24" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>30</v>
@@ -13580,14 +13583,14 @@
       </c>
       <c r="D25" s="15"/>
       <c r="E25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F25"/>
       <c r="G25" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="15"/>
@@ -16978,16 +16981,16 @@
     </row>
     <row r="32" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="D32" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>25</v>
@@ -17463,7 +17466,7 @@
       </c>
       <c r="L33" s="7"/>
       <c r="M33" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>28</v>
@@ -17477,7 +17480,7 @@
       <c r="AB33" s="7"/>
       <c r="AC33"/>
       <c r="AD33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AE33"/>
       <c r="AF33"/>
@@ -17943,7 +17946,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="11"/>
       <c r="J34" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>30</v>
@@ -17966,7 +17969,7 @@
       <c r="X34" s="7"/>
       <c r="AB34" s="7"/>
       <c r="AC34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD34"/>
       <c r="AE34"/>
@@ -18424,10 +18427,10 @@
     </row>
     <row r="35" spans="1:482" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
@@ -18445,7 +18448,7 @@
       <c r="U35" s="15"/>
       <c r="V35" s="15"/>
       <c r="W35" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X35" s="15"/>
       <c r="Y35" s="15"/>
@@ -18453,7 +18456,7 @@
       <c r="AA35" s="15"/>
       <c r="AB35" s="15"/>
       <c r="AC35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AD35"/>
       <c r="AE35"/>
@@ -18911,26 +18914,26 @@
     </row>
     <row r="36" spans="1:482" ht="34" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:482" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:482" x14ac:dyDescent="0.2">
       <c r="AD38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:482" x14ac:dyDescent="0.2">

</xml_diff>